<commit_message>
edit format data excel
</commit_message>
<xml_diff>
--- a/assets/data_dosen/format.xlsx
+++ b/assets/data_dosen/format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaenur\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\promethee\assets\data_dosen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF91993-6284-446A-BD00-119FB5F77F2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC445C5-17B9-4EC2-86E1-9A24BEEDDEF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16FD0EA6-9D4E-44AA-8B85-5CC24A387135}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>NIDN</t>
   </si>
@@ -73,27 +73,6 @@
   </si>
   <si>
     <t>X10</t>
-  </si>
-  <si>
-    <t>Zaenur</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>Laki - Laki</t>
-  </si>
-  <si>
-    <t>Rochman</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>061234513</t>
-  </si>
-  <si>
-    <t>061234516</t>
   </si>
 </sst>
 </file>
@@ -456,7 +435,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,92 +485,16 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>